<commit_message>
Change language toggles to look for "Spanish" instead of HTML. (#53)
Temporary change pending resolution of NCIOCPL/cgov-digital-platform#1541
</commit_message>
<xml_diff>
--- a/test-data/languagetoggle-data.xlsx
+++ b/test-data/languagetoggle-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/learnb/git/digiplat-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6290F03E-A612-4272-8FA3-C0DC854DB6DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A071A27D-9017-054F-A4AE-EF9077A5BF13}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6855" windowHeight="8250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20020" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_translation" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>path</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>expectedtoggle</t>
+  </si>
+  <si>
+    <t>Spanish</t>
   </si>
 </sst>
 </file>
@@ -473,16 +476,16 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.625" customWidth="1"/>
-    <col min="2" max="2" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +502,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -512,11 +515,11 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -530,10 +533,10 @@
         <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -547,10 +550,10 @@
         <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -564,10 +567,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -581,10 +584,10 @@
         <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -598,10 +601,10 @@
         <v>13</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -615,10 +618,10 @@
         <v>26</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -648,14 +651,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="29.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.125" style="3"/>
+    <col min="1" max="1" width="55.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -669,7 +672,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -680,7 +683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -691,7 +694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -702,10 +705,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
     </row>
   </sheetData>

</xml_diff>